<commit_message>
Add overlay line v1
</commit_message>
<xml_diff>
--- a/server/overlay-line/specs/overlay_line_spec.xlsx
+++ b/server/overlay-line/specs/overlay_line_spec.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="66">
   <si>
     <t>overlay_line</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>M / N</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -570,773 +573,935 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="53.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>3</v>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>41</v>
       </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>3</v>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>17</v>
       </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>3</v>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>3</v>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>3</v>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>20</v>
       </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3</v>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>23</v>
       </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>3</v>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
         <v>24</v>
       </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>3</v>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>43</v>
       </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>3</v>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
         <v>25</v>
       </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>3</v>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
         <v>26</v>
       </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>27</v>
       </c>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>3</v>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>28</v>
       </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>4</v>
-      </c>
       <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>30</v>
       </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>29</v>
       </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
       <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
         <v>31</v>
       </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>29</v>
       </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
       <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
         <v>32</v>
       </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>29</v>
       </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
       <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
         <v>33</v>
       </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>29</v>
       </c>
-      <c r="B35" t="s">
-        <v>4</v>
-      </c>
       <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>34</v>
       </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>29</v>
       </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
       <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
         <v>35</v>
       </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>29</v>
       </c>
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
       <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
         <v>36</v>
       </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>29</v>
       </c>
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
       <c r="C38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
         <v>44</v>
       </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>29</v>
       </c>
-      <c r="B39" t="s">
-        <v>3</v>
-      </c>
       <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
         <v>45</v>
       </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>29</v>
       </c>
-      <c r="B40" t="s">
-        <v>3</v>
-      </c>
       <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
         <v>46</v>
       </c>
-      <c r="D40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>29</v>
       </c>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
       <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
         <v>47</v>
       </c>
-      <c r="D41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>29</v>
       </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
       <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
         <v>48</v>
       </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>49</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>50</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>51</v>
       </c>
-      <c r="D43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>49</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>50</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>52</v>
       </c>
-      <c r="D44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
         <v>49</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>53</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>54</v>
       </c>
-      <c r="D45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
         <v>49</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>53</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>55</v>
       </c>
-      <c r="D46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
         <v>49</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>53</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>56</v>
       </c>
-      <c r="D47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>49</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>53</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>57</v>
       </c>
-      <c r="D48" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
         <v>49</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>53</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>58</v>
       </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>59</v>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>59</v>
       </c>
       <c r="C50" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" t="s">
         <v>60</v>
       </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>59</v>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>59</v>
       </c>
       <c r="C51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" t="s">
         <v>61</v>
       </c>
-      <c r="D51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>59</v>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>59</v>
       </c>
       <c r="C52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" t="s">
         <v>62</v>
       </c>
-      <c r="D52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>59</v>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>59</v>
       </c>
       <c r="C53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" t="s">
         <v>63</v>
       </c>
-      <c r="D53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>59</v>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>59</v>
       </c>
       <c r="C54" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" t="s">
         <v>64</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix pointset curveX,Y,Z deleted - Quang
</commit_message>
<xml_diff>
--- a/server/overlay-line/specs/overlay_line_spec.xlsx
+++ b/server/overlay-line/specs/overlay_line_spec.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maskx\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\UET\wi-backend\server\overlay-line\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add well header, update family cross,his,overlay template
</commit_message>
<xml_diff>
--- a/server/overlay-line/specs/overlay_line_spec.xlsx
+++ b/server/overlay-line/specs/overlay_line_spec.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\UET\wi-backend\server\overlay-line\specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\wi-backend\server\overlay-line\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516"/>
   </bookViews>
   <sheets>
     <sheet name="overlay_line" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="121">
   <si>
     <t>overlay_line</t>
   </si>
@@ -371,25 +371,22 @@
     <t>Reeves Sonic/Density Wyllie Dtf 189</t>
   </si>
   <si>
-    <t>["Apparent Matrix Density","Borehole Fluid Density","Bulk Density","Bulk Density (Array)","Bulk Density Correction","Bulk Density Hydrocarbon Corrected","Core Grain Density","Corrected ZDL Density","Density","Density (kg/m3)","Density Correction","Density Count Rate (PEF)","Density Porosity","Density Porosity Lime","Density Porosity Sand","Density Squared","Fluid Density","Fluid Density Contrast","Gas Density","Grain Density","Matrix Density","Mud Filtrate Density","Oil Density","Resolution Formation Density"]</t>
-  </si>
-  <si>
-    <t>["Neutron Porosity","Neutron Porosity Correction","Neutron Porosity Hydrocarbon Corrected","Neutron Porosity Lime","Neutron Porosity Sand","Neutron Porosity Squared","Compensated Neutron Porosity","Thermal Neutron Porosity","Thermal Neutron Porosity 1"]</t>
-  </si>
-  <si>
-    <t>["Acoustic","Acoustic (us/m)","Acoustic Attenuation Rate","Acoustic Normalization Factor"]</t>
-  </si>
-  <si>
-    <t>["Apparent Matrix Density","Borehole Fluid Density","Bulk Density","Bulk Density(Array)","Bulk Density Correction","Bulk Density Hydrocarbon Corrected","Core Grain Density","Corrected ZDL Density","Density","Density (kg/m3)","Density Correction","Density Count Rate (PEF)","Density Porosity","Density Porosity Lime","Density Porosity Sand","Density Squared","Fluid Density","Fluid Density Contrast","Gas Density","Grain Density","Matrix Density","Mud Filtrate Density","Oil Density","Resolution Formation Density"]</t>
-  </si>
-  <si>
-    <t>["Block Porosity","Compensated Neutron Porosity","Core Porosity","Core Porosity Under Stress (Array)","Density Porosity","Density Porosity Lime","Density Porosity Sand","Effective Porosity","Effective Porosity 1","Fracture Porosity","Fracture porosity cut off value for fracture basement","Isolated Porosity","Net Porosity","Net Porosity","Net Sand Fraction","Neutron Porosity","Neutron Porosity Correction","Neutron Porosity Hydrocarbon Corrected","Neutron Porosity Lime","Neutron Porosity Sand","Neutron Porosity Squared","Open Porosity","Open porosity cut off value","Parallel Porosity","Porosity","Porosity Pc Modeling","Porosity Unclipped","Secondary effective Porosity","Secondary Porosity","Secondary porosity cut off for basement reservoir","Standoff Porosity","Thermal Neutron Porosity","Thermal Neutron Porosity 1","Total Porosity","Total Porosity 1","Vug Porosity"]</t>
-  </si>
-  <si>
     <t>[]</t>
   </si>
   <si>
-    <t>["Core Permeability","Core Permeability Log10","Core Permeability Vertical","Core Permeability Under Stress (Array)","Average Permeability","Horizontal Permeability","Linear Permeability","Net Permeability","NMR Permeability","Permeability","Vertical Permeability","Permeability Pc Modeling","Permeability (nD)"]</t>
+    <t>["Apparent Matrix Density","Borehole Fluid Density","Bulk Density","Bulk Density (Array)","Bulk Density Correction","Bulk Density Hydrocarbon Corrected","Core Grain Density","Corrected ZDL Density","Density Correction","Density Count Rate","Density Porosity","Density Porosity Lime","Density Porosity Sand","Density Squared","Fluid Density","Fluid Density Contrast","Gas Density","Grain Density","Matrix Density","Mud Filtrate Density","Oil Density"]</t>
+  </si>
+  <si>
+    <t>["Neutron Porosity","Neutron Porosity Correction","Neutron Porosity Hydrocarbon Corrected","Neutron Porosity Lime","Neutron Porosity Sand","Neutron Porosity Squared","Compensated Neutron Porosity","Thermal Neutron Porosity"]</t>
+  </si>
+  <si>
+    <t>["Acoustic","Acoustic Attenuation Rate","Acoustic Normalization Factor"]</t>
+  </si>
+  <si>
+    <t>["Block Porosity","Compensated Neutron Porosity","Core Porosity","Core Porosity Under Stress (Array)","Density Porosity","Density Porosity Lime","Density Porosity Sand","Effective Porosity","Fracture Porosity","Fracture porosity cutoff - Fracture Vug Workflow","Isolated Porosity","Net Porosity","Net Porosity","Net Sand Fraction","Neutron Porosity","Neutron Porosity Correction","Neutron Porosity Hydrocarbon Corrected","Neutron Porosity Lime","Neutron Porosity Sand","Neutron Porosity Squared","Open Porosity","Open porosity cutoff - Fracture Vug Workflow","Parallel Porosity","Porosity","Porosity Pc Modeling","Porosity Unclipped","Secondary effective Porosity","Secondary Porosity","Secondary porosity cutoff - Fracture Vug Workflow","Standoff Porosity","Thermal Neutron Porosity","Total Porosity","Vug Porosity"]</t>
+  </si>
+  <si>
+    <t>["Core Permeability","Core Permeability Log10","Core Permeability Vertical","Core Permeability Under Stress (Array)","Average Permeability","Horizontal Permeability","Linear Permeability","Net Permeability","NMR Permeability","Permeability","Vertical Permeability","Permeability Pc Modeling"]</t>
   </si>
 </sst>
 </file>
@@ -425,9 +422,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,19 +740,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="53.5703125" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" customWidth="1"/>
+    <col min="2" max="2" width="67.33203125" customWidth="1"/>
+    <col min="3" max="3" width="103.44140625" customWidth="1"/>
+    <col min="4" max="4" width="53.5546875" customWidth="1"/>
+    <col min="5" max="5" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -773,15 +769,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -790,15 +786,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -807,15 +803,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
@@ -824,15 +820,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -841,15 +837,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -858,15 +854,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -875,15 +871,15 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -892,15 +888,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -909,7 +905,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -920,15 +916,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -937,15 +933,15 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D12" t="s">
         <v>44</v>
@@ -954,15 +950,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D13" t="s">
         <v>41</v>
@@ -971,15 +967,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
@@ -988,15 +984,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D15" t="s">
         <v>42</v>
@@ -1005,15 +1001,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
@@ -1022,15 +1018,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
         <v>43</v>
@@ -1039,7 +1035,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1050,15 +1046,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -1067,15 +1063,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
@@ -1084,15 +1080,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
         <v>27</v>
@@ -1101,15 +1097,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
@@ -1118,7 +1114,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1129,12 +1125,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24" t="s">
         <v>119</v>
@@ -1146,7 +1142,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1154,7 +1150,7 @@
         <v>119</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D25" t="s">
         <v>47</v>
@@ -1163,7 +1159,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1171,7 +1167,7 @@
         <v>119</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D26" t="s">
         <v>48</v>
@@ -1180,7 +1176,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1188,7 +1184,7 @@
         <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
         <v>49</v>
@@ -1197,7 +1193,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1205,7 +1201,7 @@
         <v>119</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D28" t="s">
         <v>50</v>
@@ -1214,7 +1210,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1222,7 +1218,7 @@
         <v>119</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D29" t="s">
         <v>51</v>
@@ -1231,7 +1227,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1242,15 +1238,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D31" t="s">
         <v>114</v>
@@ -1259,15 +1255,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -1276,15 +1272,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -1293,15 +1289,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
         <v>28</v>
@@ -1310,7 +1306,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1318,7 +1314,7 @@
         <v>119</v>
       </c>
       <c r="C35" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
         <v>45</v>
@@ -1327,7 +1323,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1335,7 +1331,7 @@
         <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D36" t="s">
         <v>46</v>
@@ -1344,15 +1340,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D37" t="s">
         <v>35</v>
@@ -1361,15 +1357,15 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
         <v>36</v>
@@ -1378,15 +1374,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
         <v>37</v>
@@ -1395,15 +1391,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -1412,15 +1408,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D41" t="s">
         <v>30</v>
@@ -1429,15 +1425,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D42" t="s">
         <v>29</v>
@@ -1446,15 +1442,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D43" t="s">
         <v>21</v>
@@ -1463,15 +1459,15 @@
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C44" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D44" t="s">
         <v>39</v>
@@ -1480,15 +1476,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -1497,7 +1493,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1508,15 +1504,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
@@ -1525,15 +1521,15 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>115</v>
+      <c r="B48" t="s">
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D48" t="s">
         <v>20</v>
@@ -1542,15 +1538,15 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C49" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D49" t="s">
         <v>38</v>
@@ -1559,15 +1555,15 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C50" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D50" t="s">
         <v>16</v>
@@ -1576,15 +1572,15 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C51" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
@@ -1593,15 +1589,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D52" t="s">
         <v>18</v>
@@ -1610,15 +1606,15 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C53" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D53" t="s">
         <v>14</v>
@@ -1627,15 +1623,15 @@
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D54" t="s">
         <v>15</v>
@@ -1644,15 +1640,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C55" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" t="s">
         <v>32</v>
@@ -1661,15 +1657,15 @@
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C56" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D56" t="s">
         <v>31</v>
@@ -1680,7 +1676,7 @@
     </row>
   </sheetData>
   <sortState ref="A2:E56">
-    <sortCondition ref="A1"/>
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>